<commit_message>
scaling try of p3
</commit_message>
<xml_diff>
--- a/p2_record.xlsx
+++ b/p2_record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harry\Desktop\Data-Science_HW3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9700AE26-F4F2-49CD-86DF-67D11731F1FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A13755-B71F-419B-96D5-987E23080EB1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6880" xr2:uid="{7ABFF391-5A73-46B5-A20E-98C635431F56}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="99">
   <si>
     <t xml:space="preserve">    "a = 0.3 #重視正確率(a大)或重視選少feature, a = 0~1\n",</t>
   </si>
@@ -276,10 +275,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>exp2中比例是1:2:2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>phi_p=2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -288,42 +283,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>w大</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>phi_p大</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>w小</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>w=3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>phi_p=6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>phi_g=6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>phi_p小</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>phi_g大</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>phi_g小</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>exp4.換成w_decay=True</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -353,6 +316,102 @@
   </si>
   <si>
     <t>實驗順序: exp2 -&gt; exp3 -&gt; exp4 -&gt; exp1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>exp2測得lr=5有不錯的表現</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>exp2中比例是1:1:1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>best lr=3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lr=3(用你exp2量到最好的lr)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>w大 3:1:1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>w小 1:3:3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>phi_p大 1:3:1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>phi_p小 3:1:3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>phi_g大 1:1:3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>phi_g小 3:3:1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>平均速度=0.2*3=0.6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>平均速度可寫成(0.25*w+0.25*phi_p+0.25*phi_g)=0.2=0.25*5r, r=0.16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>w=0.8*3/5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>phi_p=0.8*1/5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>phi_g=0.8*1/5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>w=0.8*1/7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>phi_p=0.8*3/7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>phi_g=0.8*3/7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>w=0.8*1/5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>phi_p=0.8*3/5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>w=0.8*3/7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>phi_p=0.8*1/7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>phi_g=0.8*3/5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>phi_g=0.8*1/7</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -719,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74335FF9-7BAA-4314-A47C-2D254B0BF3F3}">
   <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -754,7 +813,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.4">
@@ -1213,6 +1272,9 @@
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A58" t="s">
+        <v>75</v>
+      </c>
       <c r="B58" t="s">
         <v>30</v>
       </c>
@@ -1371,27 +1433,30 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
-        <v>64</v>
+        <v>76</v>
+      </c>
+      <c r="K67" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="B68" t="s">
         <v>20</v>
       </c>
       <c r="C68" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="D68" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="E68" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="F68" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="G68" t="s">
         <v>11</v>
@@ -1401,26 +1466,34 @@
       </c>
       <c r="I68" t="s">
         <v>13</v>
+      </c>
+      <c r="K68" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K69" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="B70" t="s">
         <v>20</v>
       </c>
       <c r="C70" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="D70" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="E70" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="F70" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="G70" t="s">
         <v>11</v>
@@ -1434,22 +1507,22 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="B72" t="s">
         <v>20</v>
       </c>
       <c r="C72" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="D72" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="E72" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="F72" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="G72" t="s">
         <v>11</v>
@@ -1463,22 +1536,22 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="B74" t="s">
         <v>20</v>
       </c>
       <c r="C74" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="D74" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="E74" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="F74" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="G74" t="s">
         <v>11</v>
@@ -1492,22 +1565,22 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="B76" t="s">
         <v>20</v>
       </c>
       <c r="C76" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="D76" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="E76" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="F76" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="G76" t="s">
         <v>11</v>
@@ -1521,22 +1594,22 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="B78" t="s">
         <v>20</v>
       </c>
       <c r="C78" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="D78" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="E78" t="s">
-        <v>66</v>
+        <v>98</v>
       </c>
       <c r="F78" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="G78" t="s">
         <v>11</v>
@@ -1550,10 +1623,10 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A81" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C81" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.4">
@@ -1564,13 +1637,13 @@
         <v>20</v>
       </c>
       <c r="D82" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E82" t="s">
+        <v>64</v>
+      </c>
+      <c r="F82" t="s">
         <v>65</v>
-      </c>
-      <c r="F82" t="s">
-        <v>66</v>
       </c>
       <c r="G82" t="s">
         <v>56</v>
@@ -1585,12 +1658,12 @@
         <v>13</v>
       </c>
       <c r="K82" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B84" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.4">
@@ -1598,13 +1671,13 @@
         <v>20</v>
       </c>
       <c r="D85" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E85" t="s">
+        <v>64</v>
+      </c>
+      <c r="F85" t="s">
         <v>65</v>
-      </c>
-      <c r="F85" t="s">
-        <v>66</v>
       </c>
       <c r="G85" t="s">
         <v>56</v>
@@ -1624,13 +1697,13 @@
         <v>20</v>
       </c>
       <c r="D87" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E87" t="s">
+        <v>64</v>
+      </c>
+      <c r="F87" t="s">
         <v>65</v>
-      </c>
-      <c r="F87" t="s">
-        <v>66</v>
       </c>
       <c r="G87" t="s">
         <v>56</v>
@@ -1650,13 +1723,13 @@
         <v>20</v>
       </c>
       <c r="D89" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E89" t="s">
+        <v>64</v>
+      </c>
+      <c r="F89" t="s">
         <v>65</v>
-      </c>
-      <c r="F89" t="s">
-        <v>66</v>
       </c>
       <c r="G89" t="s">
         <v>56</v>

</xml_diff>